<commit_message>
refactor: adapt validation json schema to new units
</commit_message>
<xml_diff>
--- a/test/example_import_files/exampleSensorData.xlsx
+++ b/test/example_import_files/exampleSensorData.xlsx
@@ -22,7 +22,7 @@
     <t xml:space="preserve">maxPrecision</t>
   </si>
   <si>
-    <t xml:space="preserve">timestampInMicroseconds</t>
+    <t xml:space="preserve">timestamp</t>
   </si>
   <si>
     <t xml:space="preserve">data</t>
@@ -31,13 +31,13 @@
     <t xml:space="preserve">linearAcceleration</t>
   </si>
   <si>
-    <t xml:space="preserve">metersPerSecondSquared</t>
+    <t xml:space="preserve">Acceleration.meterPerSecondSquared</t>
   </si>
   <si>
     <t xml:space="preserve">1.4, 0.0, 9.81</t>
   </si>
   <si>
-    <t xml:space="preserve">gravitationalForce</t>
+    <t xml:space="preserve">Acceleration.gravity</t>
   </si>
   <si>
     <t xml:space="preserve">0.2, 0.0, 1.0</t>

</xml_diff>